<commit_message>
Create the excel file
</commit_message>
<xml_diff>
--- a/docs/excel.xlsx
+++ b/docs/excel.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\Ynov\go\projet-red\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1002E0-6908-47A0-8042-9FCBEE7BF0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,11 +24,88 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+  <si>
+    <t>Tache</t>
+  </si>
+  <si>
+    <t>Effort</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Partie 1</t>
+  </si>
+  <si>
+    <t>Création du personnage</t>
+  </si>
+  <si>
+    <t>Initialisation du personnage</t>
+  </si>
+  <si>
+    <t>Affichage des informations du personnages</t>
+  </si>
+  <si>
+    <t>Acces à l'inventaire</t>
+  </si>
+  <si>
+    <t>Potion de vie</t>
+  </si>
+  <si>
+    <t>Marchand</t>
+  </si>
+  <si>
+    <t>Wasted!</t>
+  </si>
+  <si>
+    <t>Potion de poison</t>
+  </si>
+  <si>
+    <t>Wingardium leviosa</t>
+  </si>
+  <si>
+    <t>Amélioration de la création du personnage</t>
+  </si>
+  <si>
+    <t>Limite d'inventaire</t>
+  </si>
+  <si>
+    <t>Création du menu</t>
+  </si>
+  <si>
+    <t>optionnel 1</t>
+  </si>
+  <si>
+    <t>optionnel 2</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -37,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -45,12 +128,183 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +584,162 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="12" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="7"/>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="7"/>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="7"/>
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Base, tache 1 2 3
</commit_message>
<xml_diff>
--- a/docs/excel.xlsx
+++ b/docs/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\Ynov\go\projet-red\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1002E0-6908-47A0-8042-9FCBEE7BF0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0016B04D-69FE-4381-831C-FE1664ADB65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Tache</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>TODO</t>
+  </si>
+  <si>
+    <t>GOING</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -112,15 +118,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -248,26 +272,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -290,12 +299,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -303,6 +306,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -585,7 +597,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
@@ -595,12 +607,14 @@
   <cols>
     <col min="1" max="1" width="16.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="57.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="12" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="18.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -612,129 +626,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C2" s="11"/>
+      <c r="D2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C3" s="11"/>
+      <c r="D3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C4" s="11"/>
+      <c r="D4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C5" s="11"/>
+      <c r="D5" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C6" s="11"/>
+      <c r="D6" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C7" s="11"/>
+      <c r="D7" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C8" s="11"/>
+      <c r="D8" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C9" s="11"/>
+      <c r="D9" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C10" s="11"/>
+      <c r="D10" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C11" s="11"/>
+      <c r="D11" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C12" s="11"/>
+      <c r="D12" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="11" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="15" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Restart from nothing - task 10 OK
</commit_message>
<xml_diff>
--- a/docs/excel.xlsx
+++ b/docs/excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\Ynov\go\projet-red\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F37D74E-9178-4193-A3D9-C9E9E57D20D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0059AF77-82ED-4DA9-A58F-E66AE26A7816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>Tache</t>
   </si>
@@ -75,12 +75,6 @@
     <t>Création du menu</t>
   </si>
   <si>
-    <t>optionnel 1</t>
-  </si>
-  <si>
-    <t>optionnel 2</t>
-  </si>
-  <si>
     <t>TODO</t>
   </si>
   <si>
@@ -97,6 +91,66 @@
   </si>
   <si>
     <t>NEED IMPROVEMENT</t>
+  </si>
+  <si>
+    <t>Partie 2</t>
+  </si>
+  <si>
+    <t>Money, money, money</t>
+  </si>
+  <si>
+    <t>Two for the Price of One</t>
+  </si>
+  <si>
+    <t>Gimme! Gimme! Gimme!</t>
+  </si>
+  <si>
+    <t>Mamma Mia</t>
+  </si>
+  <si>
+    <t>On and on and on</t>
+  </si>
+  <si>
+    <t>optionnel 1.1</t>
+  </si>
+  <si>
+    <t>optionnel 1.2</t>
+  </si>
+  <si>
+    <t>optionnel 2.1</t>
+  </si>
+  <si>
+    <t>Partie 3</t>
+  </si>
+  <si>
+    <t>La Chose</t>
+  </si>
+  <si>
+    <t>Fighter Squad</t>
+  </si>
+  <si>
+    <t>A.I Intelligence artificielle</t>
+  </si>
+  <si>
+    <t>Ready Player One</t>
+  </si>
+  <si>
+    <t>Duel</t>
+  </si>
+  <si>
+    <t>Partie 4</t>
+  </si>
+  <si>
+    <t>Initiative</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>Combat magique</t>
+  </si>
+  <si>
+    <t>Ressource de mana</t>
   </si>
 </sst>
 </file>
@@ -127,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,8 +224,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -194,135 +266,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -333,38 +276,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -383,15 +300,33 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,178 +607,325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="57.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="31.85546875" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="15" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="12"/>
+      <c r="B3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="12"/>
+      <c r="B4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="12"/>
+      <c r="B5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="F5" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="12"/>
+      <c r="B6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="F6" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="12"/>
+      <c r="B7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="F7" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="12"/>
+      <c r="B8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="F8" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="12"/>
+      <c r="B9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="F9" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="12"/>
+      <c r="B10" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="F10" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="12"/>
+      <c r="B11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="21" t="s">
+      <c r="B14" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
-      <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
-      <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="23" t="s">
-        <v>18</v>
-      </c>
+      <c r="C14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="14"/>
+      <c r="B15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="14"/>
+      <c r="B16" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="14"/>
+      <c r="B17" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="16"/>
+      <c r="B20" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="16"/>
+      <c r="B21" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="16"/>
+      <c r="B22" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="16"/>
+      <c r="B23" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="22"/>
+      <c r="B25" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="22"/>
+      <c r="B26" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="22"/>
+      <c r="B27" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Remove old color library Add hand made Colorize func Clean up code
</commit_message>
<xml_diff>
--- a/docs/excel.xlsx
+++ b/docs/excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\Ynov\go\projet-red\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C48C99-3DC5-40B1-ABB5-1A32B57AA5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA2F30C-581A-4D41-8331-C24BFB882B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1410" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -685,8 +685,8 @@
       <c r="B6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>21</v>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="D6" s="4"/>
       <c r="F6" s="6" t="s">

</xml_diff>

<commit_message>
Minimal ok -> Task 20
</commit_message>
<xml_diff>
--- a/docs/excel.xlsx
+++ b/docs/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\Ynov\go\projet-red\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA2F30C-581A-4D41-8331-C24BFB882B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866299A5-CB72-45A8-8C77-06995AF640EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
   <si>
     <t>Tache</t>
   </si>
@@ -151,13 +151,19 @@
   </si>
   <si>
     <t>Ressource de mana</t>
+  </si>
+  <si>
+    <t>Auteur</t>
+  </si>
+  <si>
+    <t>BB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,8 +186,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,25 +228,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,10 +275,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -279,57 +288,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -607,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -619,315 +653,434 @@
     <col min="2" max="2" width="57.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="E1" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="12"/>
-      <c r="B3" s="17" t="s">
+      <c r="C2" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
-      <c r="B4" s="17" t="s">
+      <c r="C3" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="23">
+        <v>0</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="17" t="s">
+      <c r="C4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="23">
+        <v>0</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="F5" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="12"/>
-      <c r="B6" s="17" t="s">
+      <c r="C5" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="F6" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
-      <c r="B7" s="17" t="s">
+      <c r="C6" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="23">
+        <v>0.35</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="F7" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
-      <c r="B8" s="17" t="s">
+      <c r="C7" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="F8" s="8" t="s">
+      <c r="C8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="7"/>
+      <c r="B9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="7"/>
+      <c r="B10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="7"/>
+      <c r="B11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="12"/>
-      <c r="B9" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="F9" s="9" t="s">
+      <c r="D13" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="25">
+        <v>0</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="9"/>
+      <c r="B15" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="9"/>
+      <c r="B16" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="9"/>
+      <c r="B17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="25">
+        <v>0.15</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="12"/>
-      <c r="B10" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="F10" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="12"/>
-      <c r="B11" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="D18" s="26"/>
+      <c r="E18" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="27">
+        <v>0</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="11"/>
+      <c r="B20" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="11"/>
+      <c r="B21" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="27">
+        <v>0.05</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="11"/>
+      <c r="B22" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="11"/>
+      <c r="B23" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
-      <c r="B15" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="9" t="s">
+      <c r="D24" s="28"/>
+      <c r="E24" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="17"/>
+      <c r="B25" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
-      <c r="B16" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="D25" s="28"/>
+      <c r="E25" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="17"/>
+      <c r="B26" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
-      <c r="B17" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="9" t="s">
+      <c r="D26" s="28"/>
+      <c r="E26" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="17"/>
+      <c r="B27" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="16"/>
-      <c r="B20" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="16"/>
-      <c r="B21" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="16"/>
-      <c r="B22" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="16"/>
-      <c r="B23" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="4"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
last push, I certainly forgot something somewhere...
</commit_message>
<xml_diff>
--- a/docs/excel.xlsx
+++ b/docs/excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\projet-red\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\Ynov\go\projet-red\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DC06C2-F510-430B-AA24-BC07A4A79493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C72882-9FD2-417C-AE93-BE94E98764E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
   <si>
     <t>Tache</t>
   </si>
@@ -166,13 +166,30 @@
   </si>
   <si>
     <t>*Duel</t>
+  </si>
+  <si>
+    <t>I saw it in the mirror</t>
+  </si>
+  <si>
+    <r>
+      <t>DONE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> BUT NEED IMPROVEMENT</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,7 +234,12 @@
     </font>
     <font>
       <sz val="16"/>
-      <color theme="7" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -313,7 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -406,10 +428,16 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -696,17 +724,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y154"/>
+  <dimension ref="A1:Y155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="57.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="36"/>
@@ -815,7 +843,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="20">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>43</v>
@@ -833,7 +861,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="20">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>43</v>
@@ -884,7 +912,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="20">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>43</v>
@@ -931,7 +959,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="21">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>43</v>
@@ -944,8 +972,8 @@
       <c r="B13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="40" t="s">
-        <v>21</v>
+      <c r="C13" s="42" t="s">
+        <v>48</v>
       </c>
       <c r="D13" s="21">
         <v>0.05</v>
@@ -980,7 +1008,7 @@
         <v>18</v>
       </c>
       <c r="D15" s="22">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>43</v>
@@ -989,13 +1017,13 @@
     <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" s="8"/>
       <c r="B16" s="13" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="22">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="22" t="s">
         <v>43</v>
@@ -1004,58 +1032,58 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
       <c r="B17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="8"/>
+      <c r="B18" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="22">
-        <v>0.15</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="9" t="s">
+      <c r="C18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B19" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C19" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="10" t="s">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B20" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="24">
+      <c r="C20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="24">
         <v>0</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="10"/>
-      <c r="B20" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>46</v>
       </c>
       <c r="E20" s="24" t="s">
         <v>43</v>
@@ -1064,7 +1092,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="10"/>
       <c r="B21" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>18</v>
@@ -1079,10 +1107,10 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="10"/>
       <c r="B22" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>18</v>
+        <v>34</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>48</v>
       </c>
       <c r="D22" s="24" t="s">
         <v>46</v>
@@ -1094,59 +1122,65 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="10"/>
       <c r="B23" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="10"/>
+      <c r="B24" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="24">
-        <v>0.45</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="16" t="s">
+      <c r="C24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="24">
+        <v>0.65</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B25" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="16"/>
-      <c r="B25" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="25">
-        <v>0.1</v>
-      </c>
+      <c r="D25" s="25"/>
       <c r="E25" s="25"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="16"/>
       <c r="B26" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
+        <v>39</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="16"/>
       <c r="B27" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>16</v>
@@ -1155,28 +1189,32 @@
       <c r="E27" s="25"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="16"/>
+      <c r="B28" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B29" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="31">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E28" s="32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="28"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="32"/>
+      <c r="C29" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="28"/>
@@ -1199,12 +1237,12 @@
       <c r="D32" s="30"/>
       <c r="E32" s="32"/>
     </row>
-    <row r="33" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="33"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="32"/>
     </row>
     <row r="34" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="33"/>
@@ -2053,6 +2091,13 @@
       <c r="E154" s="36"/>
       <c r="F154" s="36"/>
     </row>
+    <row r="155" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A155" s="33"/>
+      <c r="C155" s="35"/>
+      <c r="D155" s="35"/>
+      <c r="E155" s="36"/>
+      <c r="F155" s="36"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>